<commit_message>
BOM corrections (thanks Sean!)
</commit_message>
<xml_diff>
--- a/PCB/BOM.xlsx
+++ b/PCB/BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="200">
   <si>
     <t>Refs</t>
   </si>
@@ -144,9 +144,6 @@
     <t>RAPC712X</t>
   </si>
   <si>
-    <t>878-6787</t>
-  </si>
-  <si>
     <t>Y1</t>
   </si>
   <si>
@@ -384,9 +381,6 @@
     <t>Linear</t>
   </si>
   <si>
-    <t>DC1766A-B-ND</t>
-  </si>
-  <si>
     <t>U12</t>
   </si>
   <si>
@@ -417,9 +411,6 @@
     <t>SM0805HC</t>
   </si>
   <si>
-    <t>147-9844</t>
-  </si>
-  <si>
     <t>DISABLE_FLASH1;POWER_SEL1</t>
   </si>
   <si>
@@ -552,9 +543,6 @@
     <t>STMicroelectronics</t>
   </si>
   <si>
-    <t>102-6170</t>
-  </si>
-  <si>
     <t>U10</t>
   </si>
   <si>
@@ -586,6 +574,51 @@
   </si>
   <si>
     <t>806-3964</t>
+  </si>
+  <si>
+    <t>174-9844</t>
+  </si>
+  <si>
+    <t>LTC6957IMS-4#PBF-ND</t>
+  </si>
+  <si>
+    <t>250-000</t>
+  </si>
+  <si>
+    <t>Price Per component</t>
+  </si>
+  <si>
+    <t>Price Per board</t>
+  </si>
+  <si>
+    <t>Total component cost:</t>
+  </si>
+  <si>
+    <t>Total component number:</t>
+  </si>
+  <si>
+    <t>Assembly</t>
+  </si>
+  <si>
+    <t>Manufacture</t>
+  </si>
+  <si>
+    <t>Components</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total per board</t>
+  </si>
+  <si>
+    <t>PCB Train Quotation (5 boards)</t>
+  </si>
+  <si>
+    <t>5 day + 5 day</t>
+  </si>
+  <si>
+    <t>10 day + 10 day</t>
   </si>
 </sst>
 </file>
@@ -728,7 +761,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -906,6 +939,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1069,8 +1108,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1116,7 +1159,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1130,12 +1177,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H45" totalsRowShown="0">
-  <autoFilter ref="A1:H45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J47" totalsRowShown="0">
+  <autoFilter ref="A1:J47"/>
   <sortState ref="A2:H45">
     <sortCondition ref="E1:E45"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="10">
     <tableColumn id="1" name="Refs"/>
     <tableColumn id="2" name="Value"/>
     <tableColumn id="3" name="Footprint"/>
@@ -1144,6 +1191,10 @@
     <tableColumn id="6" name="MPN"/>
     <tableColumn id="7" name="SPR"/>
     <tableColumn id="8" name="SPN"/>
+    <tableColumn id="9" name="Price Per component"/>
+    <tableColumn id="10" name="Price Per board" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1446,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,9 +1513,11 @@
     <col min="6" max="6" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1489,16 +1542,22 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>188</v>
+      </c>
+      <c r="J1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -1515,16 +1574,20 @@
       <c r="H2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1541,16 +1604,20 @@
       <c r="H3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1567,16 +1634,20 @@
       <c r="H4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D5">
         <v>13</v>
@@ -1593,16 +1664,20 @@
       <c r="H5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -1619,16 +1694,20 @@
       <c r="H6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D7">
         <v>9</v>
@@ -1645,16 +1724,20 @@
       <c r="H7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -1671,16 +1754,20 @@
       <c r="H8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -1697,16 +1784,20 @@
       <c r="H9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -1723,8 +1814,12 @@
       <c r="H10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1749,8 +1844,12 @@
       <c r="H11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1775,8 +1874,12 @@
       <c r="H12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1801,8 +1904,12 @@
       <c r="H13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1827,8 +1934,12 @@
       <c r="H14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1853,8 +1964,12 @@
       <c r="H15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1879,8 +1994,12 @@
       <c r="H16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1905,8 +2024,12 @@
       <c r="H17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1931,8 +2054,12 @@
       <c r="H18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1957,8 +2084,12 @@
       <c r="H19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1983,372 +2114,474 @@
       <c r="H20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
         <v>77</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>78</v>
-      </c>
-      <c r="C21" t="s">
-        <v>79</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" t="s">
         <v>80</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>81</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>82</v>
       </c>
-      <c r="H21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>8.52</v>
+      </c>
+      <c r="J21">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>8.52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
         <v>60</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>61</v>
-      </c>
-      <c r="C22" t="s">
-        <v>62</v>
       </c>
       <c r="D22">
         <v>3</v>
       </c>
       <c r="E22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" t="s">
         <v>63</v>
-      </c>
-      <c r="F22" t="s">
-        <v>64</v>
       </c>
       <c r="G22" t="s">
         <v>13</v>
       </c>
       <c r="H22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="I22">
+        <v>5.16</v>
+      </c>
+      <c r="J22">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" t="s">
         <v>127</v>
-      </c>
-      <c r="B23" t="s">
-        <v>128</v>
-      </c>
-      <c r="C23" t="s">
-        <v>129</v>
       </c>
       <c r="D23">
         <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G23" t="s">
         <v>13</v>
       </c>
       <c r="H23" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="I23">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="J23">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0.83199999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
         <v>54</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>55</v>
-      </c>
-      <c r="C24" t="s">
-        <v>56</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" t="s">
         <v>57</v>
-      </c>
-      <c r="F24" t="s">
-        <v>58</v>
       </c>
       <c r="G24" t="s">
         <v>13</v>
       </c>
       <c r="H24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="I24">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="J24">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0.40400000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" t="s">
         <v>122</v>
-      </c>
-      <c r="B25" t="s">
-        <v>123</v>
-      </c>
-      <c r="C25" t="s">
-        <v>124</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G25" t="s">
         <v>13</v>
       </c>
       <c r="H25" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="I25">
+        <v>3.27</v>
+      </c>
+      <c r="J25">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>3.27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B26" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C26" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F26" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G26" t="s">
         <v>13</v>
       </c>
       <c r="H26" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="I26">
+        <v>0.2</v>
+      </c>
+      <c r="J26">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" t="s">
         <v>111</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>112</v>
-      </c>
-      <c r="C27" t="s">
-        <v>113</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" t="s">
         <v>114</v>
-      </c>
-      <c r="F27" t="s">
-        <v>115</v>
       </c>
       <c r="G27" t="s">
         <v>13</v>
       </c>
       <c r="H27" t="s">
+        <v>115</v>
+      </c>
+      <c r="I27">
+        <v>1.425</v>
+      </c>
+      <c r="J27">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>1.425</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>117</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>118</v>
-      </c>
-      <c r="C28" t="s">
-        <v>119</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H28" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="I28">
+        <v>5.95</v>
+      </c>
+      <c r="J28">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
         <v>42</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>43</v>
-      </c>
-      <c r="C29" t="s">
-        <v>44</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" t="s">
         <v>45</v>
-      </c>
-      <c r="F29" t="s">
-        <v>46</v>
       </c>
       <c r="G29" t="s">
         <v>13</v>
       </c>
       <c r="H29" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29">
+        <v>1.38</v>
+      </c>
+      <c r="J29">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
         <v>48</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>49</v>
-      </c>
-      <c r="C30" t="s">
-        <v>50</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" t="s">
         <v>51</v>
-      </c>
-      <c r="F30" t="s">
-        <v>52</v>
       </c>
       <c r="G30" t="s">
         <v>13</v>
       </c>
       <c r="H30" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="I30">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="J30">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" t="s">
         <v>95</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>96</v>
-      </c>
-      <c r="C31" t="s">
-        <v>97</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
+        <v>97</v>
+      </c>
+      <c r="F31" t="s">
         <v>98</v>
-      </c>
-      <c r="F31" t="s">
-        <v>99</v>
       </c>
       <c r="G31" t="s">
         <v>13</v>
       </c>
       <c r="H31" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="I31">
+        <v>1.925</v>
+      </c>
+      <c r="J31">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>1.925</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
         <v>72</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>73</v>
-      </c>
-      <c r="C32" t="s">
-        <v>74</v>
       </c>
       <c r="D32">
         <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G32" t="s">
         <v>13</v>
       </c>
       <c r="H32" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="I32">
+        <v>3.97</v>
+      </c>
+      <c r="J32">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>23.82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
         <v>66</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>67</v>
-      </c>
-      <c r="C33" t="s">
-        <v>68</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" t="s">
         <v>69</v>
-      </c>
-      <c r="F33" t="s">
-        <v>70</v>
       </c>
       <c r="G33" t="s">
         <v>13</v>
       </c>
       <c r="H33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="I33">
+        <v>0.502</v>
+      </c>
+      <c r="J33">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0.502</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B34" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C34" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F34" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G34" t="s">
         <v>13</v>
       </c>
       <c r="H34" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="I34">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="J34">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>8.1000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -2373,16 +2606,23 @@
       <c r="H35" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>3.02</v>
+      </c>
+      <c r="J35">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B36" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C36" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -2391,68 +2631,89 @@
         <v>11</v>
       </c>
       <c r="F36" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G36" t="s">
         <v>13</v>
       </c>
       <c r="H36" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="I36">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="J36">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0.186</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B37" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C37" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F37" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G37" t="s">
         <v>13</v>
       </c>
       <c r="H37" t="s">
+        <v>169</v>
+      </c>
+      <c r="I37">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="J37">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>170</v>
+      </c>
+      <c r="B38" t="s">
+        <v>171</v>
+      </c>
+      <c r="C38" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>173</v>
-      </c>
-      <c r="B38" t="s">
-        <v>174</v>
-      </c>
-      <c r="C38" t="s">
-        <v>175</v>
       </c>
       <c r="D38">
         <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F38" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G38" t="s">
         <v>13</v>
       </c>
       <c r="H38" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="I38">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="J38">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>1.071</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -2472,166 +2733,336 @@
         <v>40</v>
       </c>
       <c r="G39" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+      <c r="H39">
+        <v>1608726</v>
+      </c>
+      <c r="I39">
+        <v>1.56</v>
+      </c>
+      <c r="J39">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B40" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C40" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D40">
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F40" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G40" t="s">
         <v>13</v>
       </c>
       <c r="H40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="I40">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="J40">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>2.3450000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" t="s">
         <v>84</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>85</v>
-      </c>
-      <c r="C41" t="s">
-        <v>86</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41" t="s">
         <v>87</v>
-      </c>
-      <c r="F41" t="s">
-        <v>88</v>
       </c>
       <c r="G41" t="s">
         <v>13</v>
       </c>
       <c r="H41" t="s">
+        <v>88</v>
+      </c>
+      <c r="I41">
+        <v>0.308</v>
+      </c>
+      <c r="J41">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0.308</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
         <v>90</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>91</v>
-      </c>
-      <c r="C42" t="s">
-        <v>92</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G42" t="s">
         <v>13</v>
       </c>
       <c r="H42" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="I42">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="J42">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0.92200000000000004</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" t="s">
         <v>101</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>102</v>
-      </c>
-      <c r="C43" t="s">
-        <v>103</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G43" t="s">
         <v>13</v>
       </c>
       <c r="H43" t="s">
+        <v>104</v>
+      </c>
+      <c r="I43">
+        <v>4.5789999999999997</v>
+      </c>
+      <c r="J43">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>4.5789999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
         <v>106</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>107</v>
-      </c>
-      <c r="C44" t="s">
-        <v>108</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G44" t="s">
         <v>13</v>
       </c>
       <c r="H44" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="I44">
+        <v>3.7050000000000001</v>
+      </c>
+      <c r="J44">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>3.7050000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B45" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C45" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F45" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G45" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H45">
         <v>8796998</v>
+      </c>
+      <c r="I45">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="J45">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0.48299999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I46" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="J46" s="4">
+        <f>SUM(J2:J45)</f>
+        <v>82.88900000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C47" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D47" s="3">
+        <f>SUM(D2:D45)</f>
+        <v>120</v>
+      </c>
+      <c r="J47" s="2">
+        <f>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Price Per component]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>193</v>
+      </c>
+      <c r="D51">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>192</v>
+      </c>
+      <c r="D52">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>194</v>
+      </c>
+      <c r="D53">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>195</v>
+      </c>
+      <c r="D54">
+        <f>SUM(D51:D53)</f>
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>196</v>
+      </c>
+      <c r="D55" s="1">
+        <f>D54/5</f>
+        <v>263</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>193</v>
+      </c>
+      <c r="D58">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>192</v>
+      </c>
+      <c r="D59">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>194</v>
+      </c>
+      <c r="D60">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>195</v>
+      </c>
+      <c r="D61">
+        <f>SUM(D58:D60)</f>
+        <v>927</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>196</v>
+      </c>
+      <c r="D62" s="1">
+        <f>D61/5</f>
+        <v>185.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>